<commit_message>
Added Email, View Template, Edit template code and test data
</commit_message>
<xml_diff>
--- a/TestingFramework/TestData/TC_10_EditTemplate.xlsx
+++ b/TestingFramework/TestData/TC_10_EditTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="945" windowWidth="14805" windowHeight="7170" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="1005" windowWidth="14805" windowHeight="7110" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="studiologin" sheetId="18" r:id="rId1"/>
@@ -2438,8 +2438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>